<commit_message>
new model with 83.5% Accuracy
</commit_message>
<xml_diff>
--- a/log/training_log.xlsx
+++ b/log/training_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,350 +482,205 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B2" t="n">
-        <v>0.66</v>
+        <v>0.83</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6212121212121212</v>
+        <v>0.84375</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6212121212121212</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6212121212121212</v>
+        <v>0.826530612244898</v>
       </c>
       <c r="F2" t="n">
-        <v>39.140625</v>
+        <v>25.28125</v>
       </c>
       <c r="G2" t="n">
-        <v>3.46875</v>
+        <v>1.46875</v>
       </c>
       <c r="H2" t="n">
-        <v>7564361728</v>
+        <v>7644233728</v>
       </c>
       <c r="I2" t="n">
-        <v>293.6384737491608</v>
+        <v>260.9365339279175</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B3" t="n">
-        <v>0.68</v>
+        <v>0.825</v>
       </c>
       <c r="C3" t="n">
-        <v>0.652542372881356</v>
+        <v>0.8350515463917526</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5661764705882353</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6062992125984251</v>
+        <v>0.8223350253807107</v>
       </c>
       <c r="F3" t="n">
-        <v>67.390625</v>
+        <v>22.21875</v>
       </c>
       <c r="G3" t="n">
-        <v>12.03125</v>
+        <v>2.59375</v>
       </c>
       <c r="H3" t="n">
-        <v>201089024</v>
+        <v>682217472</v>
       </c>
       <c r="I3" t="n">
-        <v>348.4260687828064</v>
+        <v>332.3033769130707</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>0.71</v>
+        <v>0.83</v>
       </c>
       <c r="C4" t="n">
-        <v>0.75</v>
+        <v>0.84375</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4436619718309859</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5575221238938053</v>
+        <v>0.826530612244898</v>
       </c>
       <c r="F4" t="n">
-        <v>85.96875</v>
+        <v>22.578125</v>
       </c>
       <c r="G4" t="n">
-        <v>19.078125</v>
+        <v>5.640625</v>
       </c>
       <c r="H4" t="n">
-        <v>1399287808</v>
+        <v>-2554433536</v>
       </c>
       <c r="I4" t="n">
-        <v>325.6433916091919</v>
+        <v>392.7677466869354</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>0.72</v>
+        <v>0.835</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7244897959183674</v>
+        <v>0.845360824742268</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4930555555555556</v>
+        <v>0.82</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5867768595041323</v>
+        <v>0.83248730964467</v>
       </c>
       <c r="F5" t="n">
-        <v>74.703125</v>
+        <v>21.28125</v>
       </c>
       <c r="G5" t="n">
-        <v>17.625</v>
+        <v>4.96875</v>
       </c>
       <c r="H5" t="n">
-        <v>-616329216</v>
+        <v>724201472</v>
       </c>
       <c r="I5" t="n">
-        <v>331.0578882694244</v>
+        <v>369.5096917152405</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B6" t="n">
-        <v>0.695</v>
+        <v>0.835</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7052631578947368</v>
+        <v>0.845360824742268</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4820143884892086</v>
+        <v>0.82</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5726495726495726</v>
+        <v>0.83248730964467</v>
       </c>
       <c r="F6" t="n">
-        <v>75.078125</v>
+        <v>20.703125</v>
       </c>
       <c r="G6" t="n">
-        <v>18.75</v>
+        <v>7.078125</v>
       </c>
       <c r="H6" t="n">
-        <v>-229711872</v>
+        <v>-773591040</v>
       </c>
       <c r="I6" t="n">
-        <v>356.8690690994263</v>
+        <v>407.268709897995</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B7" t="n">
-        <v>0.755</v>
+        <v>0.835</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8148148148148148</v>
+        <v>0.845360824742268</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4370860927152318</v>
+        <v>0.82</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5689655172413792</v>
+        <v>0.83248730964467</v>
       </c>
       <c r="F7" t="n">
-        <v>79.046875</v>
+        <v>20.25</v>
       </c>
       <c r="G7" t="n">
-        <v>20.03125</v>
+        <v>5.53125</v>
       </c>
       <c r="H7" t="n">
-        <v>663334912</v>
+        <v>-95969280</v>
       </c>
       <c r="I7" t="n">
-        <v>356.3517537117004</v>
+        <v>398.269159078598</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B8" t="n">
-        <v>0.73</v>
+        <v>0.835</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7948717948717948</v>
+        <v>0.845360824742268</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4246575342465753</v>
+        <v>0.82</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5535714285714286</v>
+        <v>0.83248730964467</v>
       </c>
       <c r="F8" t="n">
-        <v>80.0625</v>
+        <v>20.3125</v>
       </c>
       <c r="G8" t="n">
-        <v>19.125</v>
+        <v>7.140625</v>
       </c>
       <c r="H8" t="n">
-        <v>-389525504</v>
+        <v>195874816</v>
       </c>
       <c r="I8" t="n">
-        <v>356.0388281345367</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.735</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.7974683544303798</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.4285714285714285</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.5575221238938053</v>
-      </c>
-      <c r="F9" t="n">
-        <v>78.359375</v>
-      </c>
-      <c r="G9" t="n">
-        <v>19.3125</v>
-      </c>
-      <c r="H9" t="n">
-        <v>357249024</v>
-      </c>
-      <c r="I9" t="n">
-        <v>355.0252194404602</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.735</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.7701149425287356</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.4557823129251701</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.5726495726495727</v>
-      </c>
-      <c r="F10" t="n">
-        <v>82.8125</v>
-      </c>
-      <c r="G10" t="n">
-        <v>18.796875</v>
-      </c>
-      <c r="H10" t="n">
-        <v>189132800</v>
-      </c>
-      <c r="I10" t="n">
-        <v>351.1173505783081</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.755</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.7475728155339806</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.5099337748344371</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.6062992125984252</v>
-      </c>
-      <c r="F11" t="n">
-        <v>84.765625</v>
-      </c>
-      <c r="G11" t="n">
-        <v>20.28125</v>
-      </c>
-      <c r="H11" t="n">
-        <v>53481472</v>
-      </c>
-      <c r="I11" t="n">
-        <v>343.6342244148254</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.7555555555555555</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.4657534246575342</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.5762711864406779</v>
-      </c>
-      <c r="F12" t="n">
-        <v>94.25</v>
-      </c>
-      <c r="G12" t="n">
-        <v>20.359375</v>
-      </c>
-      <c r="H12" t="n">
-        <v>142798848</v>
-      </c>
-      <c r="I12" t="n">
-        <v>338.8581249713898</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.7307692307692307</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.5135135135135135</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.6031746031746031</v>
-      </c>
-      <c r="F13" t="n">
-        <v>86.625</v>
-      </c>
-      <c r="G13" t="n">
-        <v>20.90625</v>
-      </c>
-      <c r="H13" t="n">
-        <v>-1068863488</v>
-      </c>
-      <c r="I13" t="n">
-        <v>365.0283360481262</v>
+        <v>421.8510708808899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>